<commit_message>
DB updated on 2025-09-29 22:12:53
</commit_message>
<xml_diff>
--- a/convert.xlsx
+++ b/convert.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarva\Documents\node\Time keepers\TimeKeepersServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CA3F7A-BA72-464C-A55D-2FB5F86DB835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852C8A4A-F0C4-4E16-A56C-A2FCD4E3AF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,13 +611,13 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="1.7109375" customWidth="1"/>
     <col min="4" max="4" width="1.42578125" customWidth="1"/>
     <col min="5" max="5" width="62.140625" customWidth="1"/>
@@ -688,21 +688,21 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>75</v>
@@ -710,33 +710,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>75</v>
@@ -744,118 +744,118 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>75</v>
@@ -863,16 +863,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>75</v>
@@ -880,16 +880,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>75</v>
@@ -897,16 +897,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>75</v>
@@ -914,33 +914,33 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>75</v>
@@ -948,33 +948,33 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
         <v>75</v>
@@ -982,16 +982,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
         <v>75</v>
@@ -999,16 +999,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
         <v>75</v>
@@ -1016,16 +1016,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
         <v>75</v>
@@ -1033,16 +1033,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="E25" t="s">
         <v>75</v>

</xml_diff>